<commit_message>
Add results of expirements with dif. portion with Catboost model
</commit_message>
<xml_diff>
--- a/results_expirements/hard_experiments/0. jan22-summary/datasets_info.xlsx
+++ b/results_expirements/hard_experiments/0. jan22-summary/datasets_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\results_expirements\hard_experiments\0. jan22-summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F543578-16A5-4423-809C-1E5A2B50BD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E3A054-DAE5-4450-A26F-FDD29EC604C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17064" windowHeight="9468" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3687" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3815" uniqueCount="59">
   <si>
     <t>Dataset</t>
   </si>
@@ -12856,8 +12856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4222938A-628F-4BC6-8D87-E0D97C7DC227}">
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AM20" sqref="AM20:AR23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13559,6 +13559,66 @@
       <c r="AB8" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="AG8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:58">
       <c r="A9" t="s">
@@ -13636,65 +13696,77 @@
       <c r="AB9" s="10">
         <v>0.997999999999999</v>
       </c>
-      <c r="AG9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>39</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>35</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE9" t="s">
-        <v>38</v>
-      </c>
-      <c r="BF9" t="s">
-        <v>39</v>
+      <c r="AF9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG9">
+        <v>558.9</v>
+      </c>
+      <c r="AH9">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AI9">
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="AJ9">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN9">
+        <v>311</v>
+      </c>
+      <c r="AO9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AP9">
+        <v>0.1012</v>
+      </c>
+      <c r="AQ9">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="AR9">
+        <v>1</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU9">
+        <v>67.3</v>
+      </c>
+      <c r="AV9">
+        <v>2E-3</v>
+      </c>
+      <c r="AW9">
+        <v>4.65E-2</v>
+      </c>
+      <c r="AX9">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="AY9">
+        <v>1</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB9">
+        <v>608.6</v>
+      </c>
+      <c r="BC9">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="BD9">
+        <v>0.1477</v>
+      </c>
+      <c r="BE9">
+        <v>0.1099</v>
+      </c>
+      <c r="BF9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:58">
@@ -13771,76 +13843,76 @@
         <v>0.99309999999999998</v>
       </c>
       <c r="AF10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AG10">
-        <v>606.9</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="AH10">
-        <v>4.9999999999999897E-3</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="AI10">
-        <v>0.14449999999999999</v>
+        <v>0.80969999999999998</v>
       </c>
       <c r="AJ10">
-        <v>0.1085</v>
+        <v>0.428899999999999</v>
       </c>
       <c r="AK10">
-        <v>1</v>
+        <v>0.99229999999999996</v>
       </c>
       <c r="AM10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AN10">
-        <v>606.9</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="AO10">
-        <v>4.9999999999999897E-3</v>
+        <v>6.3399999999999998E-2</v>
       </c>
       <c r="AP10">
-        <v>0.14279999999999901</v>
+        <v>2.0030999999999999</v>
       </c>
       <c r="AQ10">
-        <v>0.10680000000000001</v>
+        <v>1.2867</v>
       </c>
       <c r="AR10">
-        <v>1</v>
+        <v>0.95679999999999998</v>
       </c>
       <c r="AT10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AU10">
-        <v>606.9</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="AV10">
-        <v>5.09999999999999E-3</v>
+        <v>0.12870000000000001</v>
       </c>
       <c r="AW10">
-        <v>0.14299999999999999</v>
+        <v>5.2219999999999898</v>
       </c>
       <c r="AX10">
-        <v>0.1074</v>
+        <v>3.23029999999999</v>
       </c>
       <c r="AY10">
-        <v>1</v>
+        <v>0.70720000000000005</v>
       </c>
       <c r="BA10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="BB10">
-        <v>606.9</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="BC10">
-        <v>4.9999999999999897E-3</v>
+        <v>1.37E-2</v>
       </c>
       <c r="BD10">
-        <v>0.1434</v>
+        <v>0.47110000000000002</v>
       </c>
       <c r="BE10">
-        <v>0.1075</v>
+        <v>0.28559999999999902</v>
       </c>
       <c r="BF10">
-        <v>1</v>
+        <v>0.99760000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:58">
@@ -13917,150 +13989,76 @@
         <v>0.99329999999999996</v>
       </c>
       <c r="AF11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AG11">
-        <v>69.099999999999994</v>
+        <v>77</v>
       </c>
       <c r="AH11">
-        <v>1.1599999999999999E-2</v>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="AI11">
-        <v>0.36399999999999999</v>
+        <v>0.78480000000000005</v>
       </c>
       <c r="AJ11">
-        <v>0.2487</v>
+        <v>0.39049999999999901</v>
       </c>
       <c r="AK11">
-        <v>0.99860000000000004</v>
+        <v>0.99480000000000002</v>
       </c>
       <c r="AM11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AN11">
-        <v>69.099999999999994</v>
+        <v>77</v>
       </c>
       <c r="AO11">
-        <v>1.3499999999999899E-2</v>
+        <v>6.2700000000000006E-2</v>
       </c>
       <c r="AP11">
-        <v>0.59599999999999898</v>
+        <v>1.5712999999999999</v>
       </c>
       <c r="AQ11">
-        <v>0.31680000000000003</v>
+        <v>1.014</v>
       </c>
       <c r="AR11">
-        <v>0.99580000000000002</v>
+        <v>0.97919999999999996</v>
       </c>
       <c r="AT11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AU11">
-        <v>69.099999999999994</v>
+        <v>77</v>
       </c>
       <c r="AV11">
-        <v>1.18E-2</v>
+        <v>0.15679999999999999</v>
       </c>
       <c r="AW11">
-        <v>0.37019999999999997</v>
+        <v>6.0909000000000004</v>
       </c>
       <c r="AX11">
-        <v>0.25190000000000001</v>
+        <v>3.8910999999999998</v>
       </c>
       <c r="AY11">
-        <v>0.99860000000000004</v>
+        <v>0.68189999999999995</v>
       </c>
       <c r="BA11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="BB11">
-        <v>69.099999999999994</v>
+        <v>77</v>
       </c>
       <c r="BC11">
-        <v>1.2E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="BD11">
-        <v>0.37469999999999998</v>
+        <v>0.5181</v>
       </c>
       <c r="BE11">
-        <v>0.25419999999999998</v>
+        <v>0.29609999999999997</v>
       </c>
       <c r="BF11">
-        <v>0.99860000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:58">
-      <c r="AF12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG12">
-        <v>77</v>
-      </c>
-      <c r="AH12">
-        <v>1.4500000000000001E-2</v>
-      </c>
-      <c r="AI12">
-        <v>0.4662</v>
-      </c>
-      <c r="AJ12">
-        <v>0.28349999999999997</v>
-      </c>
-      <c r="AK12">
-        <v>0.997999999999999</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN12">
-        <v>77</v>
-      </c>
-      <c r="AO12">
-        <v>1.8599999999999998E-2</v>
-      </c>
-      <c r="AP12">
-        <v>0.80830000000000002</v>
-      </c>
-      <c r="AQ12">
-        <v>0.43209999999999998</v>
-      </c>
-      <c r="AR12">
-        <v>0.99439999999999995</v>
-      </c>
-      <c r="AT12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU12">
-        <v>77</v>
-      </c>
-      <c r="AV12">
-        <v>1.4500000000000001E-2</v>
-      </c>
-      <c r="AW12">
-        <v>0.4723</v>
-      </c>
-      <c r="AX12">
-        <v>0.28489999999999999</v>
-      </c>
-      <c r="AY12">
-        <v>0.997999999999999</v>
-      </c>
-      <c r="BA12" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB12">
-        <v>77</v>
-      </c>
-      <c r="BC12">
-        <v>1.46E-2</v>
-      </c>
-      <c r="BD12">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="BE12">
-        <v>0.28610000000000002</v>
-      </c>
-      <c r="BF12">
-        <v>0.997999999999999</v>
+        <v>0.99759999999999904</v>
       </c>
     </row>
     <row r="13" spans="1:58">
@@ -14128,6 +14126,66 @@
       <c r="AB13" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="AG13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:58">
       <c r="A14" s="14" t="s">
@@ -14205,6 +14263,78 @@
       <c r="AB14" s="10">
         <v>0.99749999999999905</v>
       </c>
+      <c r="AF14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG14">
+        <v>606.9</v>
+      </c>
+      <c r="AH14">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AI14">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="AJ14">
+        <v>0.1085</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN14">
+        <v>606.9</v>
+      </c>
+      <c r="AO14">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AP14">
+        <v>0.14279999999999901</v>
+      </c>
+      <c r="AQ14">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="AR14">
+        <v>1</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU14">
+        <v>606.9</v>
+      </c>
+      <c r="AV14">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="AW14">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AX14">
+        <v>0.1074</v>
+      </c>
+      <c r="AY14">
+        <v>1</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB14">
+        <v>606.9</v>
+      </c>
+      <c r="BC14">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="BD14">
+        <v>0.1434</v>
+      </c>
+      <c r="BE14">
+        <v>0.1075</v>
+      </c>
+      <c r="BF14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:58">
       <c r="B15" s="9" t="s">
@@ -14279,65 +14409,77 @@
       <c r="AB15" s="20">
         <v>0.99350000000000005</v>
       </c>
-      <c r="AG15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BB15" t="s">
-        <v>35</v>
-      </c>
-      <c r="BC15" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BF15" t="s">
-        <v>39</v>
+      <c r="AF15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG15">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH15">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="AI15">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="AJ15">
+        <v>0.2487</v>
+      </c>
+      <c r="AK15">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN15">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AO15">
+        <v>1.3499999999999899E-2</v>
+      </c>
+      <c r="AP15">
+        <v>0.59599999999999898</v>
+      </c>
+      <c r="AQ15">
+        <v>0.31680000000000003</v>
+      </c>
+      <c r="AR15">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU15">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AV15">
+        <v>1.18E-2</v>
+      </c>
+      <c r="AW15">
+        <v>0.37019999999999997</v>
+      </c>
+      <c r="AX15">
+        <v>0.25190000000000001</v>
+      </c>
+      <c r="AY15">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB15">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BC15">
+        <v>1.2E-2</v>
+      </c>
+      <c r="BD15">
+        <v>0.37469999999999998</v>
+      </c>
+      <c r="BE15">
+        <v>0.25419999999999998</v>
+      </c>
+      <c r="BF15">
+        <v>0.99860000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:58">
@@ -14414,150 +14556,76 @@
         <v>0.99390000000000001</v>
       </c>
       <c r="AF16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AG16">
-        <v>590.9</v>
+        <v>77</v>
       </c>
       <c r="AH16">
-        <v>5.09999999999999E-3</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="AI16">
-        <v>0.14849999999999999</v>
+        <v>0.4662</v>
       </c>
       <c r="AJ16">
-        <v>0.1119</v>
+        <v>0.28349999999999997</v>
       </c>
       <c r="AK16">
-        <v>1</v>
+        <v>0.997999999999999</v>
       </c>
       <c r="AM16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AN16">
-        <v>590.9</v>
+        <v>77</v>
       </c>
       <c r="AO16">
-        <v>4.9999999999999897E-3</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="AP16">
-        <v>0.13639999999999999</v>
+        <v>0.80830000000000002</v>
       </c>
       <c r="AQ16">
-        <v>0.1031</v>
+        <v>0.43209999999999998</v>
       </c>
       <c r="AR16">
-        <v>1</v>
+        <v>0.99439999999999995</v>
       </c>
       <c r="AT16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AU16">
-        <v>590.9</v>
+        <v>77</v>
       </c>
       <c r="AV16">
-        <v>5.1999999999999902E-3</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="AW16">
-        <v>0.1452</v>
+        <v>0.4723</v>
       </c>
       <c r="AX16">
-        <v>0.10969999999999901</v>
+        <v>0.28489999999999999</v>
       </c>
       <c r="AY16">
-        <v>1</v>
+        <v>0.997999999999999</v>
       </c>
       <c r="BA16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BB16">
-        <v>590.9</v>
+        <v>77</v>
       </c>
       <c r="BC16">
-        <v>4.9999999999999897E-3</v>
+        <v>1.46E-2</v>
       </c>
       <c r="BD16">
-        <v>0.14179999999999901</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="BE16">
-        <v>0.1065</v>
+        <v>0.28610000000000002</v>
       </c>
       <c r="BF16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:58">
-      <c r="AF17" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG17">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="AH17">
-        <v>1.21E-2</v>
-      </c>
-      <c r="AI17">
-        <v>0.36449999999999999</v>
-      </c>
-      <c r="AJ17">
-        <v>0.25290000000000001</v>
-      </c>
-      <c r="AK17">
-        <v>0.99860000000000004</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN17">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="AO17">
-        <v>1.5100000000000001E-2</v>
-      </c>
-      <c r="AP17">
-        <v>0.77869999999999995</v>
-      </c>
-      <c r="AQ17">
-        <v>0.37879999999999903</v>
-      </c>
-      <c r="AR17">
-        <v>0.99259999999999904</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU17">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="AV17">
-        <v>1.21999999999999E-2</v>
-      </c>
-      <c r="AW17">
-        <v>0.37869999999999998</v>
-      </c>
-      <c r="AX17">
-        <v>0.26119999999999999</v>
-      </c>
-      <c r="AY17">
-        <v>0.99860000000000004</v>
-      </c>
-      <c r="BA17" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB17">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="BC17">
-        <v>1.18E-2</v>
-      </c>
-      <c r="BD17">
-        <v>0.36940000000000001</v>
-      </c>
-      <c r="BE17">
-        <v>0.25280000000000002</v>
-      </c>
-      <c r="BF17">
-        <v>0.99850000000000005</v>
+        <v>0.997999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:58">
@@ -14625,77 +14693,65 @@
       <c r="AB18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AF18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG18">
-        <v>77</v>
-      </c>
-      <c r="AH18">
-        <v>1.47E-2</v>
-      </c>
-      <c r="AI18">
-        <v>0.4723</v>
-      </c>
-      <c r="AJ18">
-        <v>0.288299999999999</v>
-      </c>
-      <c r="AK18">
-        <v>0.997999999999999</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN18">
-        <v>77</v>
-      </c>
-      <c r="AO18">
-        <v>2.2399999999999899E-2</v>
-      </c>
-      <c r="AP18">
-        <v>1.1935</v>
-      </c>
-      <c r="AQ18">
-        <v>0.59870000000000001</v>
-      </c>
-      <c r="AR18">
-        <v>0.98819999999999997</v>
-      </c>
-      <c r="AT18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU18">
-        <v>77</v>
-      </c>
-      <c r="AV18">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="AW18">
-        <v>0.48109999999999897</v>
-      </c>
-      <c r="AX18">
-        <v>0.29110000000000003</v>
-      </c>
-      <c r="AY18">
-        <v>0.997999999999999</v>
-      </c>
-      <c r="BA18" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB18">
-        <v>77</v>
-      </c>
-      <c r="BC18">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="BD18">
-        <v>0.47360000000000002</v>
-      </c>
-      <c r="BE18">
-        <v>0.28609999999999902</v>
-      </c>
-      <c r="BF18">
-        <v>0.997999999999999</v>
+      <c r="AG18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:58">
@@ -14774,6 +14830,78 @@
       <c r="AB19" s="10">
         <v>0.99739999999999995</v>
       </c>
+      <c r="AF19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG19">
+        <v>590.9</v>
+      </c>
+      <c r="AH19">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="AI19">
+        <v>0.14849999999999999</v>
+      </c>
+      <c r="AJ19">
+        <v>0.1119</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN19">
+        <v>590.9</v>
+      </c>
+      <c r="AO19">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AP19">
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="AQ19">
+        <v>0.1031</v>
+      </c>
+      <c r="AR19">
+        <v>1</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU19">
+        <v>590.9</v>
+      </c>
+      <c r="AV19">
+        <v>5.1999999999999902E-3</v>
+      </c>
+      <c r="AW19">
+        <v>0.1452</v>
+      </c>
+      <c r="AX19">
+        <v>0.10969999999999901</v>
+      </c>
+      <c r="AY19">
+        <v>1</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB19">
+        <v>590.9</v>
+      </c>
+      <c r="BC19">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="BD19">
+        <v>0.14179999999999901</v>
+      </c>
+      <c r="BE19">
+        <v>0.1065</v>
+      </c>
+      <c r="BF19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:58">
       <c r="B20" s="9" t="s">
@@ -14848,65 +14976,77 @@
       <c r="AB20" s="20">
         <v>0.99319999999999997</v>
       </c>
-      <c r="AG20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ20" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX20" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY20" t="s">
-        <v>39</v>
-      </c>
-      <c r="BB20" t="s">
-        <v>35</v>
-      </c>
-      <c r="BC20" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD20" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE20" t="s">
-        <v>38</v>
-      </c>
-      <c r="BF20" t="s">
-        <v>39</v>
+      <c r="AF20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG20">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH20">
+        <v>1.21E-2</v>
+      </c>
+      <c r="AI20">
+        <v>0.36449999999999999</v>
+      </c>
+      <c r="AJ20">
+        <v>0.25290000000000001</v>
+      </c>
+      <c r="AK20">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN20">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AO20">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="AP20">
+        <v>0.77869999999999995</v>
+      </c>
+      <c r="AQ20">
+        <v>0.37879999999999903</v>
+      </c>
+      <c r="AR20">
+        <v>0.99259999999999904</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU20">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AV20">
+        <v>1.21999999999999E-2</v>
+      </c>
+      <c r="AW20">
+        <v>0.37869999999999998</v>
+      </c>
+      <c r="AX20">
+        <v>0.26119999999999999</v>
+      </c>
+      <c r="AY20">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="BA20" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB20">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BC20">
+        <v>1.18E-2</v>
+      </c>
+      <c r="BD20">
+        <v>0.36940000000000001</v>
+      </c>
+      <c r="BE20">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="BF20">
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:58">
@@ -14983,150 +15123,76 @@
         <v>0.99399999999999999</v>
       </c>
       <c r="AF21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AG21">
-        <v>575.9</v>
+        <v>77</v>
       </c>
       <c r="AH21">
-        <v>4.9999999999999897E-3</v>
+        <v>1.47E-2</v>
       </c>
       <c r="AI21">
-        <v>0.1469</v>
+        <v>0.4723</v>
       </c>
       <c r="AJ21">
-        <v>0.1103</v>
+        <v>0.288299999999999</v>
       </c>
       <c r="AK21">
-        <v>1</v>
+        <v>0.997999999999999</v>
       </c>
       <c r="AM21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AN21">
-        <v>575.9</v>
+        <v>77</v>
       </c>
       <c r="AO21">
-        <v>5.1999999999999902E-3</v>
+        <v>2.2399999999999899E-2</v>
       </c>
       <c r="AP21">
-        <v>0.1358</v>
+        <v>1.1935</v>
       </c>
       <c r="AQ21">
-        <v>0.1028</v>
+        <v>0.59870000000000001</v>
       </c>
       <c r="AR21">
-        <v>1</v>
+        <v>0.98819999999999997</v>
       </c>
       <c r="AT21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AU21">
-        <v>575.9</v>
+        <v>77</v>
       </c>
       <c r="AV21">
-        <v>5.09999999999999E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AW21">
-        <v>0.14249999999999999</v>
+        <v>0.48109999999999897</v>
       </c>
       <c r="AX21">
-        <v>0.10780000000000001</v>
+        <v>0.29110000000000003</v>
       </c>
       <c r="AY21">
-        <v>1</v>
+        <v>0.997999999999999</v>
       </c>
       <c r="BA21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BB21">
-        <v>575.9</v>
+        <v>77</v>
       </c>
       <c r="BC21">
-        <v>4.9999999999999897E-3</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="BD21">
-        <v>0.13769999999999999</v>
+        <v>0.47360000000000002</v>
       </c>
       <c r="BE21">
-        <v>0.1036</v>
+        <v>0.28609999999999902</v>
       </c>
       <c r="BF21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:58">
-      <c r="AF22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG22">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="AH22">
-        <v>1.23E-2</v>
-      </c>
-      <c r="AI22">
-        <v>0.38169999999999998</v>
-      </c>
-      <c r="AJ22">
-        <v>0.26129999999999998</v>
-      </c>
-      <c r="AK22">
-        <v>0.99860000000000004</v>
-      </c>
-      <c r="AM22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN22">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="AO22">
-        <v>2.4699999999999899E-2</v>
-      </c>
-      <c r="AP22">
-        <v>1.8058999999999901</v>
-      </c>
-      <c r="AQ22">
-        <v>0.73839999999999995</v>
-      </c>
-      <c r="AR22">
-        <v>0.95639999999999903</v>
-      </c>
-      <c r="AT22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU22">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="AV22">
-        <v>1.21999999999999E-2</v>
-      </c>
-      <c r="AW22">
-        <v>0.37340000000000001</v>
-      </c>
-      <c r="AX22">
-        <v>0.25929999999999997</v>
-      </c>
-      <c r="AY22">
-        <v>0.99860000000000004</v>
-      </c>
-      <c r="BA22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB22">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="BC22">
-        <v>1.16999999999999E-2</v>
-      </c>
-      <c r="BD22">
-        <v>0.37890000000000001</v>
-      </c>
-      <c r="BE22">
-        <v>0.25679999999999997</v>
-      </c>
-      <c r="BF22">
-        <v>0.99850000000000005</v>
+        <v>0.997999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:58">
@@ -15194,77 +15260,65 @@
       <c r="AB23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AF23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG23">
-        <v>77</v>
-      </c>
-      <c r="AH23">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="AI23">
-        <v>0.48010000000000003</v>
-      </c>
-      <c r="AJ23">
-        <v>0.2954</v>
-      </c>
-      <c r="AK23">
-        <v>0.997999999999999</v>
-      </c>
-      <c r="AM23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN23">
-        <v>77</v>
-      </c>
-      <c r="AO23">
-        <v>3.61E-2</v>
-      </c>
-      <c r="AP23">
-        <v>2.6101999999999999</v>
-      </c>
-      <c r="AQ23">
-        <v>1.1559999999999999</v>
-      </c>
-      <c r="AR23">
-        <v>0.93759999999999999</v>
-      </c>
-      <c r="AT23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU23">
-        <v>77</v>
-      </c>
-      <c r="AV23">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="AW23">
-        <v>0.48209999999999997</v>
-      </c>
-      <c r="AX23">
-        <v>0.29449999999999998</v>
-      </c>
-      <c r="AY23">
-        <v>0.997999999999999</v>
-      </c>
-      <c r="BA23" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB23">
-        <v>77</v>
-      </c>
-      <c r="BC23">
-        <v>1.46E-2</v>
-      </c>
-      <c r="BD23">
-        <v>0.47010000000000002</v>
-      </c>
-      <c r="BE23">
-        <v>0.28310000000000002</v>
-      </c>
-      <c r="BF23">
-        <v>0.997999999999999</v>
+      <c r="AG23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC23" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD23" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE23" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF23" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:58">
@@ -15343,6 +15397,78 @@
       <c r="AB24" s="10">
         <v>0.99719999999999998</v>
       </c>
+      <c r="AF24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG24">
+        <v>575.9</v>
+      </c>
+      <c r="AH24">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AI24">
+        <v>0.1469</v>
+      </c>
+      <c r="AJ24">
+        <v>0.1103</v>
+      </c>
+      <c r="AK24">
+        <v>1</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN24">
+        <v>575.9</v>
+      </c>
+      <c r="AO24">
+        <v>5.1999999999999902E-3</v>
+      </c>
+      <c r="AP24">
+        <v>0.1358</v>
+      </c>
+      <c r="AQ24">
+        <v>0.1028</v>
+      </c>
+      <c r="AR24">
+        <v>1</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU24">
+        <v>575.9</v>
+      </c>
+      <c r="AV24">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="AW24">
+        <v>0.14249999999999999</v>
+      </c>
+      <c r="AX24">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="AY24">
+        <v>1</v>
+      </c>
+      <c r="BA24" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB24">
+        <v>575.9</v>
+      </c>
+      <c r="BC24">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="BD24">
+        <v>0.13769999999999999</v>
+      </c>
+      <c r="BE24">
+        <v>0.1036</v>
+      </c>
+      <c r="BF24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:58">
       <c r="B25" s="9" t="s">
@@ -15417,6 +15543,78 @@
       <c r="AB25" s="20">
         <v>0.99329999999999996</v>
       </c>
+      <c r="AF25" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG25">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH25">
+        <v>1.23E-2</v>
+      </c>
+      <c r="AI25">
+        <v>0.38169999999999998</v>
+      </c>
+      <c r="AJ25">
+        <v>0.26129999999999998</v>
+      </c>
+      <c r="AK25">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN25">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AO25">
+        <v>2.4699999999999899E-2</v>
+      </c>
+      <c r="AP25">
+        <v>1.8058999999999901</v>
+      </c>
+      <c r="AQ25">
+        <v>0.73839999999999995</v>
+      </c>
+      <c r="AR25">
+        <v>0.95639999999999903</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU25">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AV25">
+        <v>1.21999999999999E-2</v>
+      </c>
+      <c r="AW25">
+        <v>0.37340000000000001</v>
+      </c>
+      <c r="AX25">
+        <v>0.25929999999999997</v>
+      </c>
+      <c r="AY25">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="BA25" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB25">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BC25">
+        <v>1.16999999999999E-2</v>
+      </c>
+      <c r="BD25">
+        <v>0.37890000000000001</v>
+      </c>
+      <c r="BE25">
+        <v>0.25679999999999997</v>
+      </c>
+      <c r="BF25">
+        <v>0.99850000000000005</v>
+      </c>
     </row>
     <row r="26" spans="1:58">
       <c r="B26" s="11" t="s">
@@ -15490,6 +15688,78 @@
       </c>
       <c r="AB26" s="13">
         <v>0.99339999999999995</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG26">
+        <v>77</v>
+      </c>
+      <c r="AH26">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="AI26">
+        <v>0.48010000000000003</v>
+      </c>
+      <c r="AJ26">
+        <v>0.2954</v>
+      </c>
+      <c r="AK26">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN26">
+        <v>77</v>
+      </c>
+      <c r="AO26">
+        <v>3.61E-2</v>
+      </c>
+      <c r="AP26">
+        <v>2.6101999999999999</v>
+      </c>
+      <c r="AQ26">
+        <v>1.1559999999999999</v>
+      </c>
+      <c r="AR26">
+        <v>0.93759999999999999</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU26">
+        <v>77</v>
+      </c>
+      <c r="AV26">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="AW26">
+        <v>0.48209999999999997</v>
+      </c>
+      <c r="AX26">
+        <v>0.29449999999999998</v>
+      </c>
+      <c r="AY26">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="BA26" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB26">
+        <v>77</v>
+      </c>
+      <c r="BC26">
+        <v>1.46E-2</v>
+      </c>
+      <c r="BD26">
+        <v>0.47010000000000002</v>
+      </c>
+      <c r="BE26">
+        <v>0.28310000000000002</v>
+      </c>
+      <c r="BF26">
+        <v>0.997999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:58">
@@ -15557,6 +15827,66 @@
       <c r="AB28" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="AG28" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN28" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR28" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX28" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY28" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB28" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC28" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD28" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE28" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF28" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="29" spans="1:58">
       <c r="A29" s="14" t="s">
@@ -15634,6 +15964,78 @@
       <c r="AB29" s="10">
         <v>0.99709999999999999</v>
       </c>
+      <c r="AF29" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG29">
+        <v>559.9</v>
+      </c>
+      <c r="AH29">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="AI29">
+        <v>0.1487</v>
+      </c>
+      <c r="AJ29">
+        <v>0.1118</v>
+      </c>
+      <c r="AK29">
+        <v>1</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN29">
+        <v>559.9</v>
+      </c>
+      <c r="AO29">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AP29">
+        <v>0.1326</v>
+      </c>
+      <c r="AQ29">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="AR29">
+        <v>1</v>
+      </c>
+      <c r="AT29" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU29">
+        <v>559.9</v>
+      </c>
+      <c r="AV29">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AW29">
+        <v>0.142899999999999</v>
+      </c>
+      <c r="AX29">
+        <v>0.1079</v>
+      </c>
+      <c r="AY29">
+        <v>1</v>
+      </c>
+      <c r="BA29" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB29">
+        <v>559.9</v>
+      </c>
+      <c r="BC29">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="BD29">
+        <v>0.1394</v>
+      </c>
+      <c r="BE29">
+        <v>0.1041</v>
+      </c>
+      <c r="BF29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:58">
       <c r="B30" s="9" t="s">
@@ -15708,6 +16110,78 @@
       <c r="AB30" s="20">
         <v>0.99299999999999999</v>
       </c>
+      <c r="AF30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG30">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH30">
+        <v>1.21999999999999E-2</v>
+      </c>
+      <c r="AI30">
+        <v>0.3669</v>
+      </c>
+      <c r="AJ30">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="AK30">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN30">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AO30">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="AP30">
+        <v>2.5157999999999898</v>
+      </c>
+      <c r="AQ30">
+        <v>0.94389999999999996</v>
+      </c>
+      <c r="AR30">
+        <v>0.92979999999999996</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU30">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AV30">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="AW30">
+        <v>0.38929999999999998</v>
+      </c>
+      <c r="AX30">
+        <v>0.26790000000000003</v>
+      </c>
+      <c r="AY30">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="BA30" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB30">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BC30">
+        <v>1.21999999999999E-2</v>
+      </c>
+      <c r="BD30">
+        <v>0.3831</v>
+      </c>
+      <c r="BE30">
+        <v>0.26369999999999999</v>
+      </c>
+      <c r="BF30">
+        <v>0.99850000000000005</v>
+      </c>
     </row>
     <row r="31" spans="1:58">
       <c r="B31" s="11" t="s">
@@ -15782,8 +16256,80 @@
       <c r="AB31" s="13">
         <v>0.99339999999999995</v>
       </c>
-    </row>
-    <row r="33" spans="1:28">
+      <c r="AF31" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG31">
+        <v>77</v>
+      </c>
+      <c r="AH31">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="AI31">
+        <v>0.47070000000000001</v>
+      </c>
+      <c r="AJ31">
+        <v>0.29149999999999998</v>
+      </c>
+      <c r="AK31">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN31">
+        <v>77</v>
+      </c>
+      <c r="AO31">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="AP31">
+        <v>3.7671999999999999</v>
+      </c>
+      <c r="AQ31">
+        <v>1.6664999999999901</v>
+      </c>
+      <c r="AR31">
+        <v>0.88049999999999995</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU31">
+        <v>77</v>
+      </c>
+      <c r="AV31">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AW31">
+        <v>0.48649999999999999</v>
+      </c>
+      <c r="AX31">
+        <v>0.29430000000000001</v>
+      </c>
+      <c r="AY31">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="BA31" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB31">
+        <v>77</v>
+      </c>
+      <c r="BC31">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="BD31">
+        <v>0.48149999999999998</v>
+      </c>
+      <c r="BE31">
+        <v>0.289799999999999</v>
+      </c>
+      <c r="BF31">
+        <v>0.997999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:58">
       <c r="B33" s="6"/>
       <c r="C33" s="7" t="s">
         <v>35</v>
@@ -15848,8 +16394,68 @@
       <c r="AB33" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:28">
+      <c r="AG33" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ33" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV33" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX33" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY33" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB33" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC33" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD33" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE33" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:58">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -15925,8 +16531,80 @@
       <c r="AB34" s="10">
         <v>0.997</v>
       </c>
-    </row>
-    <row r="35" spans="1:28">
+      <c r="AF34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG34">
+        <v>528.9</v>
+      </c>
+      <c r="AH34">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="AI34">
+        <v>0.15140000000000001</v>
+      </c>
+      <c r="AJ34">
+        <v>0.1143</v>
+      </c>
+      <c r="AK34">
+        <v>1</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN34">
+        <v>528.9</v>
+      </c>
+      <c r="AO34">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AP34">
+        <v>0.1242</v>
+      </c>
+      <c r="AQ34">
+        <v>9.35E-2</v>
+      </c>
+      <c r="AR34">
+        <v>1</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU34">
+        <v>528.9</v>
+      </c>
+      <c r="AV34">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AW34">
+        <v>0.13980000000000001</v>
+      </c>
+      <c r="AX34">
+        <v>0.1055</v>
+      </c>
+      <c r="AY34">
+        <v>1</v>
+      </c>
+      <c r="BA34" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB34">
+        <v>528.9</v>
+      </c>
+      <c r="BC34">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="BD34">
+        <v>0.13669999999999999</v>
+      </c>
+      <c r="BE34">
+        <v>0.1031</v>
+      </c>
+      <c r="BF34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:58">
       <c r="B35" s="9" t="s">
         <v>41</v>
       </c>
@@ -15999,8 +16677,80 @@
       <c r="AB35" s="20">
         <v>0.9919</v>
       </c>
-    </row>
-    <row r="36" spans="1:28">
+      <c r="AF35" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG35">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH35">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="AI35">
+        <v>0.37959999999999999</v>
+      </c>
+      <c r="AJ35">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AK35">
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN35">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AO35">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="AP35">
+        <v>2.4718</v>
+      </c>
+      <c r="AQ35">
+        <v>1.0362</v>
+      </c>
+      <c r="AR35">
+        <v>0.93379999999999996</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU35">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AV35">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="AW35">
+        <v>0.40389999999999998</v>
+      </c>
+      <c r="AX35">
+        <v>0.27999999999999903</v>
+      </c>
+      <c r="AY35">
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="BA35" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB35">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BC35">
+        <v>1.29E-2</v>
+      </c>
+      <c r="BD35">
+        <v>0.4083</v>
+      </c>
+      <c r="BE35">
+        <v>0.27960000000000002</v>
+      </c>
+      <c r="BF35">
+        <v>0.99829999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:58">
       <c r="B36" s="11" t="s">
         <v>42</v>
       </c>
@@ -16073,8 +16823,80 @@
       <c r="AB36" s="13">
         <v>0.99179999999999902</v>
       </c>
-    </row>
-    <row r="38" spans="1:28">
+      <c r="AF36" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG36">
+        <v>77</v>
+      </c>
+      <c r="AH36">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="AI36">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="AJ36">
+        <v>0.3044</v>
+      </c>
+      <c r="AK36">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN36">
+        <v>77</v>
+      </c>
+      <c r="AO36">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="AP36">
+        <v>3.6900999999999899</v>
+      </c>
+      <c r="AQ36">
+        <v>1.76809999999999</v>
+      </c>
+      <c r="AR36">
+        <v>0.88539999999999996</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU36">
+        <v>77</v>
+      </c>
+      <c r="AV36">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="AW36">
+        <v>0.49790000000000001</v>
+      </c>
+      <c r="AX36">
+        <v>0.30459999999999998</v>
+      </c>
+      <c r="AY36">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="BA36" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB36">
+        <v>77</v>
+      </c>
+      <c r="BC36">
+        <v>1.54E-2</v>
+      </c>
+      <c r="BD36">
+        <v>0.5</v>
+      </c>
+      <c r="BE36">
+        <v>0.30459999999999998</v>
+      </c>
+      <c r="BF36">
+        <v>0.997999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:58">
       <c r="B38" s="6"/>
       <c r="C38" s="7" t="s">
         <v>35</v>
@@ -16139,8 +16961,68 @@
       <c r="AB38" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:28">
+      <c r="AG38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR38" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY38" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB38" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC38" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD38" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE38" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:58">
       <c r="A39" s="14" t="s">
         <v>49</v>
       </c>
@@ -16216,8 +17098,80 @@
       <c r="AB39" s="10">
         <v>0.99680000000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:28">
+      <c r="AF39" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG39">
+        <v>497.9</v>
+      </c>
+      <c r="AH39">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AI39">
+        <v>0.1555</v>
+      </c>
+      <c r="AJ39">
+        <v>0.1181</v>
+      </c>
+      <c r="AK39">
+        <v>1</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN39">
+        <v>497.9</v>
+      </c>
+      <c r="AO39">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AP39">
+        <v>0.12089999999999999</v>
+      </c>
+      <c r="AQ39">
+        <v>9.0799999999999895E-2</v>
+      </c>
+      <c r="AR39">
+        <v>1</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU39">
+        <v>497.9</v>
+      </c>
+      <c r="AV39">
+        <v>4.9999999999999897E-3</v>
+      </c>
+      <c r="AW39">
+        <v>0.13969999999999999</v>
+      </c>
+      <c r="AX39">
+        <v>0.1047</v>
+      </c>
+      <c r="AY39">
+        <v>1</v>
+      </c>
+      <c r="BA39" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB39">
+        <v>497.9</v>
+      </c>
+      <c r="BC39">
+        <v>5.09999999999999E-3</v>
+      </c>
+      <c r="BD39">
+        <v>0.13679999999999901</v>
+      </c>
+      <c r="BE39">
+        <v>0.1032</v>
+      </c>
+      <c r="BF39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:58">
       <c r="B40" s="9" t="s">
         <v>41</v>
       </c>
@@ -16290,8 +17244,80 @@
       <c r="AB40" s="20">
         <v>0.99099999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:28">
+      <c r="AF40" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG40">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH40">
+        <v>1.33999999999999E-2</v>
+      </c>
+      <c r="AI40">
+        <v>0.39190000000000003</v>
+      </c>
+      <c r="AJ40">
+        <v>0.27389999999999998</v>
+      </c>
+      <c r="AK40">
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN40">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AO40">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="AP40">
+        <v>2.2194999999999898</v>
+      </c>
+      <c r="AQ40">
+        <v>1.0518999999999901</v>
+      </c>
+      <c r="AR40">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU40">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AV40">
+        <v>1.35999999999999E-2</v>
+      </c>
+      <c r="AW40">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="AX40">
+        <v>0.29110000000000003</v>
+      </c>
+      <c r="AY40">
+        <v>0.99780000000000002</v>
+      </c>
+      <c r="BA40" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB40">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BC40">
+        <v>1.34E-2</v>
+      </c>
+      <c r="BD40">
+        <v>0.43819999999999998</v>
+      </c>
+      <c r="BE40">
+        <v>0.29949999999999999</v>
+      </c>
+      <c r="BF40">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:58">
       <c r="B41" s="11" t="s">
         <v>42</v>
       </c>
@@ -16363,6 +17389,78 @@
       </c>
       <c r="AB41" s="13">
         <v>0.99099999999999999</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG41">
+        <v>77</v>
+      </c>
+      <c r="AH41">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="AI41">
+        <v>0.4864</v>
+      </c>
+      <c r="AJ41">
+        <v>0.30059999999999998</v>
+      </c>
+      <c r="AK41">
+        <v>0.997999999999999</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN41">
+        <v>77</v>
+      </c>
+      <c r="AO41">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="AP41">
+        <v>3.0670999999999999</v>
+      </c>
+      <c r="AQ41">
+        <v>1.6105</v>
+      </c>
+      <c r="AR41">
+        <v>0.92110000000000003</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU41">
+        <v>77</v>
+      </c>
+      <c r="AV41">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AW41">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="AX41">
+        <v>0.30919999999999997</v>
+      </c>
+      <c r="AY41">
+        <v>0.99789999999999901</v>
+      </c>
+      <c r="BA41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB41">
+        <v>77</v>
+      </c>
+      <c r="BC41">
+        <v>1.61E-2</v>
+      </c>
+      <c r="BD41">
+        <v>0.53139999999999998</v>
+      </c>
+      <c r="BE41">
+        <v>0.3251</v>
+      </c>
+      <c r="BF41">
+        <v>0.99769999999999903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>